<commit_message>
excel measurement template updated
</commit_message>
<xml_diff>
--- a/StateOfPractice/Peter-Notes/MeasurementTemplateInspection.xlsx
+++ b/StateOfPractice/Peter-Notes/MeasurementTemplateInspection.xlsx
@@ -31,10 +31,10 @@
     <t xml:space="preserve">Is this metric unambiguous? (yes, no*) (* if ambiguous, the reviewer should add text to say how)</t>
   </si>
   <si>
+    <t xml:space="preserve">Is this metric actually likely to be measurable? (yes, no*) (* if no, the reviewer should say why it is unlikely to be measurable)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Should this metric be removed? (yes*, no) (* if yes please state reasoning)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is this metric actually likely to be measurable? (yes, no*) (* if no, the reviewer should say why it is unlikely to be measurable)</t>
   </si>
   <si>
     <t xml:space="preserve">Are there any missing possible measurement values? (yes*, no) (* if yes, the reviewer should say what is missing)</t>
@@ -574,18 +574,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -663,11 +657,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -675,7 +669,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -687,11 +681,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -733,7 +727,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -756,10 +750,10 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">

</xml_diff>